<commit_message>
single test phase success for create change request
</commit_message>
<xml_diff>
--- a/data_driver/Change_Requirement.xlsx
+++ b/data_driver/Change_Requirement.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AutoBotBMCRemedy\data_driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\AutoBotBMCRemedy\data_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371E65CE-1073-492C-98C4-947D1C21DC25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572D2C43-01AD-439E-B738-44E62DA8BCEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1501,7 +1501,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="B2" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44041</v>
+        <v>44053</v>
       </c>
       <c r="C2" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
@@ -1608,189 +1608,189 @@
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44041</v>
-      </c>
-      <c r="C3" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C3" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D3" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Legacy</v>
-      </c>
-      <c r="E3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E3" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>New Link instalation</v>
-      </c>
-      <c r="F3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F3" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>NGSNG07,NGSNG57</v>
-      </c>
-      <c r="G3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G3" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J3" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka South</v>
+        <v>0</v>
       </c>
       <c r="K3" s="31"/>
-      <c r="L3" s="31" t="str">
+      <c r="L3" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44041</v>
-      </c>
-      <c r="C4" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C4" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D4" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Operational</v>
-      </c>
-      <c r="E4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E4" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>PAT activity</v>
-      </c>
-      <c r="F4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F4" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>SYSDRB6,SYSDRA8</v>
-      </c>
-      <c r="G4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
-      </c>
-      <c r="J4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J4" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
+        <v>0</v>
       </c>
       <c r="K4" s="31"/>
-      <c r="L4" s="31" t="str">
+      <c r="L4" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44041</v>
-      </c>
-      <c r="C5" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C5" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D5" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>DHAKA_MODERNIZATION</v>
-      </c>
-      <c r="E5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E5" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v xml:space="preserve">RAU Release Udate </v>
-      </c>
-      <c r="F5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F5" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHKHL05,DHKHL74</v>
-      </c>
-      <c r="G5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J5" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>0</v>
       </c>
       <c r="K5" s="31"/>
-      <c r="L5" s="31" t="str">
+      <c r="L5" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44041</v>
-      </c>
-      <c r="C6" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C6" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>NCCD AbisoIP</v>
-      </c>
-      <c r="E6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E6" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Dismantle activity</v>
-      </c>
-      <c r="F6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F6" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>SYGWN10,SYGWN13,SYGWN05,SYGWN01,SYSDR34</v>
-      </c>
-      <c r="G6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G6" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
-      </c>
-      <c r="J6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J6" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
+        <v>0</v>
       </c>
       <c r="K6" s="31"/>
-      <c r="L6" s="31" t="str">
+      <c r="L6" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Testing Passed for Create Change Request
</commit_message>
<xml_diff>
--- a/data_driver/Change_Requirement.xlsx
+++ b/data_driver/Change_Requirement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\AutoBotBMCRemedy\data_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA20AF9A-7D9C-41F9-AA3F-0AB2CDFD7A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B51E97-A2CC-4178-BD97-001E493DCAD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,14 +33,6 @@
     <definedName name="Sylhet">Information!$Y$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1501,7 +1493,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,44 +1557,44 @@
       </c>
       <c r="B2" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44049</v>
+        <v>44054</v>
       </c>
       <c r="C2" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
+        <v>Prodip Biswas</v>
       </c>
       <c r="D2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
+        <v>L18CellAdd, Y2020</v>
       </c>
       <c r="E2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Configuration</v>
+        <v>GSM &amp; RRU Swap</v>
       </c>
       <c r="F2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>TNDDR05,TNDDR15,TNKLH15,TNKLH16,TNMDP29</v>
+        <v>MBKLR17,SYBLG15,BMSDR14</v>
       </c>
       <c r="G2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
+        <v>Service Effective</v>
       </c>
       <c r="H2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
+        <v>00:30 Minute</v>
       </c>
       <c r="I2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Mymensingh</v>
+        <v>Sylhet</v>
       </c>
       <c r="J2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Mymensingh</v>
+        <v>e.co_Sylhet</v>
       </c>
       <c r="K2" s="31"/>
       <c r="L2" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>Sumon Kumar Biswas</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1612,31 +1604,31 @@
       </c>
       <c r="B3" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44049</v>
+        <v>44054</v>
       </c>
       <c r="C3" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
+        <v>Md. Rashekul Islam Raju</v>
       </c>
       <c r="D3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
+        <v>Project 964</v>
       </c>
       <c r="E3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Configuration</v>
+        <v>GSM Antenna Optimization</v>
       </c>
       <c r="F3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHMDP42,DHMDP47,DHMJH47,DHPTN16,DHPTN29,DHRMN04,DHRMN16,DHRMN26,DHRMN36</v>
+        <v>DHSBB16</v>
       </c>
       <c r="G3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
+        <v>Service Effective</v>
       </c>
       <c r="H3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
+        <v>00:45 Minute</v>
       </c>
       <c r="I3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
@@ -1659,7 +1651,7 @@
       </c>
       <c r="B4" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44049</v>
+        <v>44054</v>
       </c>
       <c r="C4" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
@@ -1675,11 +1667,11 @@
       </c>
       <c r="F4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>MGGHR11,MGSBL11,MGSTR01,MNLHG02,MNLHG17,GPSDRS5,MNSDR46</v>
+        <v>TNDDR05,TNDDR15,TNKLH15,TNKLH16,TNMDP29</v>
       </c>
       <c r="G4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
+        <v>Non-Service Effective</v>
       </c>
       <c r="H4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
@@ -1687,11 +1679,11 @@
       </c>
       <c r="I4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
+        <v>Mymensingh</v>
       </c>
       <c r="J4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka North</v>
+        <v>e.co_Mymensingh</v>
       </c>
       <c r="K4" s="31"/>
       <c r="L4" s="31" t="str">
@@ -1702,283 +1694,283 @@
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="29">
+        <v>44054</v>
+      </c>
+      <c r="C5" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="30">
+        <v>KM Jiaul Islam Jibon</v>
+      </c>
+      <c r="D5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="30">
+        <v>Dhaka-Modernization</v>
+      </c>
+      <c r="E5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="30">
+        <v>FE Configuration</v>
+      </c>
+      <c r="F5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="30">
+        <v>DHMDP42,DHMDP47,DHMJH47,DHPTN16,DHPTN29,DHRMN04,DHRMN16,DHRMN26,DHRMN36</v>
+      </c>
+      <c r="G5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="30">
+        <v>Non-Service Effective</v>
+      </c>
+      <c r="H5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="30">
+        <v>00:00 Minute</v>
+      </c>
+      <c r="I5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="30">
+        <v>Dhaka</v>
+      </c>
+      <c r="J5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Dhaka Metro</v>
       </c>
       <c r="K5" s="31"/>
-      <c r="L5" s="31">
+      <c r="L5" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="29">
+        <v>44054</v>
+      </c>
+      <c r="C6" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="30">
+        <v>KM Jiaul Islam Jibon</v>
+      </c>
+      <c r="D6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="30">
+        <v>Dhaka-Modernization</v>
+      </c>
+      <c r="E6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="30">
+        <v>FE Configuration</v>
+      </c>
+      <c r="F6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="30">
+        <v>MGGHR11,MGSBL11,MGSTR01,MNLHG02,MNLHG17,GPSDRS5,MNSDR46</v>
+      </c>
+      <c r="G6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="30">
+        <v>Non-Service Effective</v>
+      </c>
+      <c r="H6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="30">
+        <v>00:00 Minute</v>
+      </c>
+      <c r="I6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="30">
+        <v>Dhaka</v>
+      </c>
+      <c r="J6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Dhaka North</v>
       </c>
       <c r="K6" s="31"/>
-      <c r="L6" s="31">
+      <c r="L6" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="29">
+        <v>44054</v>
+      </c>
+      <c r="C7" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="30">
+        <v>KM Jiaul Islam Jibon</v>
+      </c>
+      <c r="D7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="30">
+        <v xml:space="preserve">CEP_OEPX </v>
+      </c>
+      <c r="E7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="30">
+        <v>FE Configuration &amp; GE Shifting</v>
+      </c>
+      <c r="F7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="30">
+        <v>DHDHN07,DHRMN09</v>
+      </c>
+      <c r="G7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="30">
+        <v>Service Effective</v>
+      </c>
+      <c r="H7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="30">
+        <v>00:30 Minute</v>
+      </c>
+      <c r="I7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="30">
+        <v>Dhaka</v>
+      </c>
+      <c r="J7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Dhaka Metro</v>
       </c>
       <c r="K7" s="31"/>
-      <c r="L7" s="31">
+      <c r="L7" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="29">
+        <v>44054</v>
+      </c>
+      <c r="C8" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="30">
+        <v>Md. Masudur Rahman</v>
+      </c>
+      <c r="D8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="30">
+        <v>Padma_Colo</v>
+      </c>
+      <c r="E8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="30">
+        <v>Rectification</v>
+      </c>
+      <c r="F8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="30">
+        <v>HGBNC04,HGNBG05</v>
+      </c>
+      <c r="G8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="30">
+        <v>Service Effective</v>
+      </c>
+      <c r="H8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="30">
+        <v>00:30 Minute</v>
+      </c>
+      <c r="I8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="30">
+        <v>Sylhet</v>
+      </c>
+      <c r="J8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Sylhet</v>
       </c>
       <c r="K8" s="31"/>
-      <c r="L8" s="31">
+      <c r="L8" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="29">
+        <v>44054</v>
+      </c>
+      <c r="C9" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="30">
+        <v>Md. Masudur Rahman</v>
+      </c>
+      <c r="D9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="30">
+        <v>DHAKA_MODERNIZATION</v>
+      </c>
+      <c r="E9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="30">
+        <v>Rectification</v>
+      </c>
+      <c r="F9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="30">
+        <v>TNGPL01,TNGTL27</v>
+      </c>
+      <c r="G9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="30">
+        <v>Service Effective</v>
+      </c>
+      <c r="H9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="30">
+        <v>00:30 Minute</v>
+      </c>
+      <c r="I9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="30">
+        <v>Mymensingh</v>
+      </c>
+      <c r="J9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Mymensingh</v>
       </c>
       <c r="K9" s="31"/>
-      <c r="L9" s="31">
+      <c r="L9" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="29">
+        <v>44054</v>
+      </c>
+      <c r="C10" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="30">
+        <v>Md. Masudur Rahman</v>
+      </c>
+      <c r="D10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="30">
+        <v>NCCD AbisoIP</v>
+      </c>
+      <c r="E10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="30">
+        <v>Dismantle activity</v>
+      </c>
+      <c r="F10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="30">
+        <v>SYGWN10,SYGWN13,SYGWN01,SYBNB02,SYSDR34,SYSDR08,SYSDR07,SYSDR13,SYSDR86,SYSDR43</v>
+      </c>
+      <c r="G10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="30">
+        <v>Non-Service Effective</v>
+      </c>
+      <c r="H10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="30">
+        <v>00:00 Minute</v>
+      </c>
+      <c r="I10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="30">
+        <v>Sylhet</v>
+      </c>
+      <c r="J10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Sylhet</v>
       </c>
       <c r="K10" s="31"/>
-      <c r="L10" s="31">
+      <c r="L10" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
All tested working for now
</commit_message>
<xml_diff>
--- a/data_driver/Change_Requirement.xlsx
+++ b/data_driver/Change_Requirement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\AutoBotBMCRemedy\data_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B51E97-A2CC-4178-BD97-001E493DCAD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6BEF3E-6153-4147-86B3-A1E12F30BA57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1493,7 +1493,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,27 +1561,27 @@
       </c>
       <c r="C2" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Prodip Biswas</v>
+        <v>Md. Masudur Rahman</v>
       </c>
       <c r="D2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>L18CellAdd, Y2020</v>
+        <v>NCCD AbisoIP</v>
       </c>
       <c r="E2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>GSM &amp; RRU Swap</v>
+        <v>Dismantle activity</v>
       </c>
       <c r="F2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>MBKLR17,SYBLG15,BMSDR14</v>
+        <v>SYSDRD4,SYDKS28,SYGLP01,SYSDR86,SYSDR43,SYSDRC2</v>
       </c>
       <c r="G2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
+        <v>Non-Service Effective</v>
       </c>
       <c r="H2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
+        <v>00:00 Minute</v>
       </c>
       <c r="I2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
@@ -1594,383 +1594,383 @@
       <c r="K2" s="31"/>
       <c r="L2" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Sumon Kumar Biswas</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44054</v>
-      </c>
-      <c r="C3" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C3" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Rashekul Islam Raju</v>
-      </c>
-      <c r="D3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D3" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Project 964</v>
-      </c>
-      <c r="E3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E3" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>GSM Antenna Optimization</v>
-      </c>
-      <c r="F3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F3" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHSBB16</v>
-      </c>
-      <c r="G3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G3" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:45 Minute</v>
-      </c>
-      <c r="I3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J3" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>0</v>
       </c>
       <c r="K3" s="31"/>
-      <c r="L3" s="31" t="str">
+      <c r="L3" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44054</v>
-      </c>
-      <c r="C4" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C4" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
-      </c>
-      <c r="D4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D4" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
-      </c>
-      <c r="E4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E4" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Configuration</v>
-      </c>
-      <c r="F4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F4" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>TNDDR05,TNDDR15,TNKLH15,TNKLH16,TNMDP29</v>
-      </c>
-      <c r="G4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Mymensingh</v>
-      </c>
-      <c r="J4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J4" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Mymensingh</v>
+        <v>0</v>
       </c>
       <c r="K4" s="31"/>
-      <c r="L4" s="31" t="str">
+      <c r="L4" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44054</v>
-      </c>
-      <c r="C5" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C5" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
-      </c>
-      <c r="D5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D5" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
-      </c>
-      <c r="E5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E5" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Configuration</v>
-      </c>
-      <c r="F5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F5" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHMDP42,DHMDP47,DHMJH47,DHPTN16,DHPTN29,DHRMN04,DHRMN16,DHRMN26,DHRMN36</v>
-      </c>
-      <c r="G5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J5" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>0</v>
       </c>
       <c r="K5" s="31"/>
-      <c r="L5" s="31" t="str">
+      <c r="L5" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44054</v>
-      </c>
-      <c r="C6" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C6" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
-      </c>
-      <c r="D6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
-      </c>
-      <c r="E6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E6" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Configuration</v>
-      </c>
-      <c r="F6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F6" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>MGGHR11,MGSBL11,MGSTR01,MNLHG02,MNLHG17,GPSDRS5,MNSDR46</v>
-      </c>
-      <c r="G6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G6" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J6" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka North</v>
+        <v>0</v>
       </c>
       <c r="K6" s="31"/>
-      <c r="L6" s="31" t="str">
+      <c r="L6" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B7" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44054</v>
-      </c>
-      <c r="C7" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C7" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
-      </c>
-      <c r="D7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D7" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v xml:space="preserve">CEP_OEPX </v>
-      </c>
-      <c r="E7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E7" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Configuration &amp; GE Shifting</v>
-      </c>
-      <c r="F7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHDHN07,DHRMN09</v>
-      </c>
-      <c r="G7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G7" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H7" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J7" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>0</v>
       </c>
       <c r="K7" s="31"/>
-      <c r="L7" s="31" t="str">
+      <c r="L7" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B8" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44054</v>
-      </c>
-      <c r="C8" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C8" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D8" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Padma_Colo</v>
-      </c>
-      <c r="E8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E8" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Rectification</v>
-      </c>
-      <c r="F8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F8" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>HGBNC04,HGNBG05</v>
-      </c>
-      <c r="G8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G8" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H8" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I8" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
-      </c>
-      <c r="J8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J8" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
+        <v>0</v>
       </c>
       <c r="K8" s="31"/>
-      <c r="L8" s="31" t="str">
+      <c r="L8" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B9" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44054</v>
-      </c>
-      <c r="C9" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C9" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D9" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>DHAKA_MODERNIZATION</v>
-      </c>
-      <c r="E9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E9" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Rectification</v>
-      </c>
-      <c r="F9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F9" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>TNGPL01,TNGTL27</v>
-      </c>
-      <c r="G9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G9" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H9" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I9" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Mymensingh</v>
-      </c>
-      <c r="J9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J9" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Mymensingh</v>
+        <v>0</v>
       </c>
       <c r="K9" s="31"/>
-      <c r="L9" s="31" t="str">
+      <c r="L9" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B10" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44054</v>
-      </c>
-      <c r="C10" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C10" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D10" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>NCCD AbisoIP</v>
-      </c>
-      <c r="E10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E10" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Dismantle activity</v>
-      </c>
-      <c r="F10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F10" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>SYGWN10,SYGWN13,SYGWN01,SYBNB02,SYSDR34,SYSDR08,SYSDR07,SYSDR13,SYSDR86,SYSDR43</v>
-      </c>
-      <c r="G10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G10" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H10" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I10" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
-      </c>
-      <c r="J10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J10" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
+        <v>0</v>
       </c>
       <c r="K10" s="31"/>
-      <c r="L10" s="31" t="str">
+      <c r="L10" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed StaleElementReferenceException on Close Function
</commit_message>
<xml_diff>
--- a/data_driver/Change_Requirement.xlsx
+++ b/data_driver/Change_Requirement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\AutoBotBMCRemedy\data_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC4B5EE-6996-422A-BE84-C81ECDA2DFA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D171A97-D89F-483A-8ACF-DF07BA3710A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1493,7 +1493,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,31 +1557,31 @@
       </c>
       <c r="B2" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44059</v>
+        <v>44073</v>
       </c>
       <c r="C2" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
+        <v>Md. Shahadat Hossain</v>
       </c>
       <c r="D2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>NCCD AbisoIP</v>
+        <v>Padma Colocation Project</v>
       </c>
       <c r="E2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>E1 Deletion</v>
+        <v>CPRI Cable &amp; RRU Swap 1/1</v>
       </c>
       <c r="F2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>SNSDR01,SNSDR03,SYBLG05,SYBNB20,SYBNB40,SYBSW07,SYKNG02,SYSDRA7,SNSDR22,SNSDR25</v>
+        <v>         SNDRI02,SNDRI05,SNDRI06,SNDRI07,SNDRI10</v>
       </c>
       <c r="G2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
+        <v>Service Effective</v>
       </c>
       <c r="H2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
+        <v>04:00 Hour</v>
       </c>
       <c r="I2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>

</xml_diff>

<commit_message>
Relationship Site Tagging working Now in Create New CR
</commit_message>
<xml_diff>
--- a/data_driver/Change_Requirement.xlsx
+++ b/data_driver/Change_Requirement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\AutoBotBMCRemedy\data_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32C636F-F28C-4CD6-9F6B-070E322BFD85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C0036D-DE40-4427-96FA-F9CB29575521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="1215" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change_List" sheetId="1" r:id="rId1"/>
@@ -1493,7 +1493,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,11 +1577,11 @@
       </c>
       <c r="G2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
+        <v>Service Effective</v>
       </c>
       <c r="H2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
+        <v>00:30 Minute</v>
       </c>
       <c r="I2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
@@ -1600,189 +1600,189 @@
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44074</v>
-      </c>
-      <c r="C3" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C3" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D3" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>CEP</v>
-      </c>
-      <c r="E3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E3" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>New Link installation</v>
-      </c>
-      <c r="F3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F3" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHBDDA7,DHTEJ15,DHTEJ07</v>
-      </c>
-      <c r="G3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G3" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J3" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>0</v>
       </c>
       <c r="K3" s="31"/>
-      <c r="L3" s="31" t="str">
+      <c r="L3" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44074</v>
-      </c>
-      <c r="C4" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C4" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D4" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Padma_Colo</v>
-      </c>
-      <c r="E4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E4" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>New Link installation</v>
-      </c>
-      <c r="F4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F4" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>BHCFN02,BHCFN26,BHLMN01,BHLMN15</v>
-      </c>
-      <c r="G4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Barisal</v>
-      </c>
-      <c r="J4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J4" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Barisal</v>
+        <v>0</v>
       </c>
       <c r="K4" s="31"/>
-      <c r="L4" s="31" t="str">
+      <c r="L4" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44074</v>
-      </c>
-      <c r="C5" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C5" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D5" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>NCCD AbisoIP</v>
-      </c>
-      <c r="E5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E5" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Traffic Check for Traffic shiftng</v>
-      </c>
-      <c r="F5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F5" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>HGNBG28,HGNBG08</v>
-      </c>
-      <c r="G5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
-      </c>
-      <c r="J5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J5" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
+        <v>0</v>
       </c>
       <c r="K5" s="31"/>
-      <c r="L5" s="31" t="str">
+      <c r="L5" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44074</v>
-      </c>
-      <c r="C6" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C6" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>CEP</v>
-      </c>
-      <c r="E6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E6" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>New Link installation</v>
-      </c>
-      <c r="F6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F6" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHMDP30,DHMDP39</v>
-      </c>
-      <c r="G6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G6" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J6" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>0</v>
       </c>
       <c r="K6" s="31"/>
-      <c r="L6" s="31" t="str">
+      <c r="L6" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working Adding Relationship for Service Effective NCR
</commit_message>
<xml_diff>
--- a/data_driver/Change_Requirement.xlsx
+++ b/data_driver/Change_Requirement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\AutoBotBMCRemedy\data_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C0036D-DE40-4427-96FA-F9CB29575521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A07BCFE-F11B-4669-BC6C-7DF42365D62A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1177,8 +1177,8 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1493,7 +1493,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B2" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="C2" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
@@ -1565,15 +1565,15 @@
       </c>
       <c r="D2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>DHAKA_MODERNIZATION</v>
+        <v>NCCD AbisoIP</v>
       </c>
       <c r="E2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>New Link installation</v>
+        <v>Garbage E1 Deletetion</v>
       </c>
       <c r="F2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>MGSNG08,DHKGNT1</v>
+        <v>SYGLP01,SYBLG09,SYBLG04</v>
       </c>
       <c r="G2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
@@ -1585,11 +1585,11 @@
       </c>
       <c r="I2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
+        <v>Sylhet</v>
       </c>
       <c r="J2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka North</v>
+        <v>e.co_Sylhet</v>
       </c>
       <c r="K2" s="31"/>
       <c r="L2" s="31" t="str">
@@ -1600,377 +1600,377 @@
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="29">
+        <v>44076</v>
+      </c>
+      <c r="C3" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="30">
+        <v>Md. Masudur Rahman</v>
+      </c>
+      <c r="D3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="30">
+        <v>CEP</v>
+      </c>
+      <c r="E3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="30">
+        <v>New Link installation</v>
+      </c>
+      <c r="F3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="30">
+        <v>DHTEJ15,DHTEJ07</v>
+      </c>
+      <c r="G3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="30">
+        <v>Service Effective</v>
+      </c>
+      <c r="H3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="30">
+        <v>00:30 Minute</v>
+      </c>
+      <c r="I3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="30">
+        <v>Dhaka</v>
+      </c>
+      <c r="J3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Dhaka Metro</v>
       </c>
       <c r="K3" s="31"/>
-      <c r="L3" s="31">
+      <c r="L3" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="29">
+        <v>44076</v>
+      </c>
+      <c r="C4" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="30">
+        <v>Md. Masudur Rahman</v>
+      </c>
+      <c r="D4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="30">
+        <v>DHAKA_MODERNIZATION</v>
+      </c>
+      <c r="E4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="30">
+        <v>Rectification</v>
+      </c>
+      <c r="F4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="30">
+        <v>TNSKP18,TNMZP48</v>
+      </c>
+      <c r="G4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="30">
+        <v>Non-Service Effective</v>
+      </c>
+      <c r="H4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="30">
+        <v>00:00 Minute</v>
+      </c>
+      <c r="I4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="30">
+        <v>Mymensingh</v>
+      </c>
+      <c r="J4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Mymensingh</v>
       </c>
       <c r="K4" s="31"/>
-      <c r="L4" s="31">
+      <c r="L4" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="29">
+        <v>44076</v>
+      </c>
+      <c r="C5" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="30">
+        <v>Md. Masudur Rahman</v>
+      </c>
+      <c r="D5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="30">
+        <v>Padma_Colo</v>
+      </c>
+      <c r="E5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="30">
+        <v>New Link installation</v>
+      </c>
+      <c r="F5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="30">
+        <v>BHCFN02,BHCFN26,BHLMN01,BHLMN15</v>
+      </c>
+      <c r="G5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="30">
+        <v>Non-Service Effective</v>
+      </c>
+      <c r="H5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="30">
+        <v>00:00 Minute</v>
+      </c>
+      <c r="I5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="30">
+        <v>Barisal</v>
+      </c>
+      <c r="J5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Barisal</v>
       </c>
       <c r="K5" s="31"/>
-      <c r="L5" s="31">
+      <c r="L5" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="29">
+        <v>44076</v>
+      </c>
+      <c r="C6" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="30">
+        <v>Md. Masudur Rahman</v>
+      </c>
+      <c r="D6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="30">
+        <v>DHAKA_MODERNIZATION</v>
+      </c>
+      <c r="E6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="30">
+        <v>New Link installation</v>
+      </c>
+      <c r="F6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="30">
+        <v>MNLHG18,MNSRN18</v>
+      </c>
+      <c r="G6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="30">
+        <v>Non-Service Effective</v>
+      </c>
+      <c r="H6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="30">
+        <v>00:00 Minute</v>
+      </c>
+      <c r="I6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="30">
+        <v>Dhaka</v>
+      </c>
+      <c r="J6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Dhaka South</v>
       </c>
       <c r="K6" s="31"/>
-      <c r="L6" s="31">
+      <c r="L6" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="29">
+        <v>44076</v>
+      </c>
+      <c r="C7" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="30">
+        <v>Md. Masudur Rahman</v>
+      </c>
+      <c r="D7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="30">
+        <v>NCCD AbisoIP</v>
+      </c>
+      <c r="E7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="30">
+        <v>Traffic Check for Traffic shiftng</v>
+      </c>
+      <c r="F7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="30">
+        <v>HGNBG28,HGNBG08</v>
+      </c>
+      <c r="G7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="30">
+        <v>Service Effective</v>
+      </c>
+      <c r="H7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="30">
+        <v>00:30 Minute</v>
+      </c>
+      <c r="I7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="30">
+        <v>Sylhet</v>
+      </c>
+      <c r="J7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Sylhet</v>
       </c>
       <c r="K7" s="31"/>
-      <c r="L7" s="31">
+      <c r="L7" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="29">
+        <v>44076</v>
+      </c>
+      <c r="C8" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="30">
+        <v>Md. Masudur Rahman</v>
+      </c>
+      <c r="D8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="30">
+        <v>DHAKA_MODERNIZATION</v>
+      </c>
+      <c r="E8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="30">
+        <v>HW upgradation</v>
+      </c>
+      <c r="F8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="30">
+        <v>GPSDR86,GPSDR42</v>
+      </c>
+      <c r="G8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="30">
+        <v>Service Effective</v>
+      </c>
+      <c r="H8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="30">
+        <v>00:30 Minute</v>
+      </c>
+      <c r="I8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="30">
+        <v>Dhaka</v>
+      </c>
+      <c r="J8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Dhaka North</v>
       </c>
       <c r="K8" s="31"/>
-      <c r="L8" s="31">
+      <c r="L8" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="29">
+        <v>44076</v>
+      </c>
+      <c r="C9" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="30">
+        <v>KM Jiaul Islam Jibon</v>
+      </c>
+      <c r="D9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="30">
+        <v>Dhaka-Modernization</v>
+      </c>
+      <c r="E9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="30">
+        <v>FE Configuration</v>
+      </c>
+      <c r="F9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="30">
+        <v>DHDHN45,DHKHL47,DHKHLA0,DHPTN29,DHRMN04,DHRMN16,DHRMN26,DHBDD78,DHGULF5,DHMDP01</v>
+      </c>
+      <c r="G9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="30">
+        <v>Non-Service Effective</v>
+      </c>
+      <c r="H9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="30">
+        <v>00:00 Minute</v>
+      </c>
+      <c r="I9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="30">
+        <v>Dhaka</v>
+      </c>
+      <c r="J9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Dhaka Metro</v>
       </c>
       <c r="K9" s="31"/>
-      <c r="L9" s="31">
+      <c r="L9" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="29">
+        <v>44076</v>
+      </c>
+      <c r="C10" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="30">
+        <v>KM Jiaul Islam Jibon</v>
+      </c>
+      <c r="D10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="30">
+        <v>Dhaka-Modernization</v>
+      </c>
+      <c r="E10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="30">
+        <v>FE Configuration</v>
+      </c>
+      <c r="F10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="30">
+        <v>MGGHR11,MGSBL11,MGSTR01,MNLHG02,MNLHG17,GPSDRS5,MNSDR46,DHSVRG5</v>
+      </c>
+      <c r="G10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="30">
+        <v>Non-Service Effective</v>
+      </c>
+      <c r="H10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="30">
+        <v>00:00 Minute</v>
+      </c>
+      <c r="I10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="30">
+        <v>Dhaka</v>
+      </c>
+      <c r="J10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>0</v>
+        <v>e.co_Dhaka North</v>
       </c>
       <c r="K10" s="31"/>
-      <c r="L10" s="31">
+      <c r="L10" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>0</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change Manager K.M Khairul Basar Added
</commit_message>
<xml_diff>
--- a/data_driver/Change_Requirement.xlsx
+++ b/data_driver/Change_Requirement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\AutoBotBMCRemedy\data_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A07BCFE-F11B-4669-BC6C-7DF42365D62A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB53C33-815A-4602-8D98-02FA7D734C1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change_List" sheetId="1" r:id="rId1"/>
@@ -1177,8 +1177,8 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1493,7 +1493,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,23 +1557,23 @@
       </c>
       <c r="B2" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44076</v>
+        <v>44079</v>
       </c>
       <c r="C2" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
+        <v>Md. Shahadat Hossain</v>
       </c>
       <c r="D2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>NCCD AbisoIP</v>
+        <v>Padma_Colo</v>
       </c>
       <c r="E2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Garbage E1 Deletetion</v>
+        <v>CPRI Cable &amp; RRU Swap 1/1</v>
       </c>
       <c r="F2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>SYGLP01,SYBLG09,SYBLG04</v>
+        <v>SNCTK27</v>
       </c>
       <c r="G2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="H2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
+        <v>04:00 Hour</v>
       </c>
       <c r="I2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
@@ -1594,383 +1594,383 @@
       <c r="K2" s="31"/>
       <c r="L2" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>K.M Khairul Bashar</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44076</v>
-      </c>
-      <c r="C3" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C3" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D3" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>CEP</v>
-      </c>
-      <c r="E3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E3" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>New Link installation</v>
-      </c>
-      <c r="F3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F3" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHTEJ15,DHTEJ07</v>
-      </c>
-      <c r="G3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G3" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J3" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J3" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>0</v>
       </c>
       <c r="K3" s="31"/>
-      <c r="L3" s="31" t="str">
+      <c r="L3" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44076</v>
-      </c>
-      <c r="C4" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C4" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D4" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>DHAKA_MODERNIZATION</v>
-      </c>
-      <c r="E4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E4" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Rectification</v>
-      </c>
-      <c r="F4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F4" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>TNSKP18,TNMZP48</v>
-      </c>
-      <c r="G4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Mymensingh</v>
-      </c>
-      <c r="J4" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J4" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Mymensingh</v>
+        <v>0</v>
       </c>
       <c r="K4" s="31"/>
-      <c r="L4" s="31" t="str">
+      <c r="L4" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44076</v>
-      </c>
-      <c r="C5" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C5" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D5" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Padma_Colo</v>
-      </c>
-      <c r="E5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E5" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>New Link installation</v>
-      </c>
-      <c r="F5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F5" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>BHCFN02,BHCFN26,BHLMN01,BHLMN15</v>
-      </c>
-      <c r="G5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Barisal</v>
-      </c>
-      <c r="J5" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J5" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Barisal</v>
+        <v>0</v>
       </c>
       <c r="K5" s="31"/>
-      <c r="L5" s="31" t="str">
+      <c r="L5" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44076</v>
-      </c>
-      <c r="C6" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C6" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>DHAKA_MODERNIZATION</v>
-      </c>
-      <c r="E6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E6" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>New Link installation</v>
-      </c>
-      <c r="F6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F6" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>MNLHG18,MNSRN18</v>
-      </c>
-      <c r="G6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G6" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J6" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J6" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka South</v>
+        <v>0</v>
       </c>
       <c r="K6" s="31"/>
-      <c r="L6" s="31" t="str">
+      <c r="L6" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B7" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44076</v>
-      </c>
-      <c r="C7" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C7" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D7" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>NCCD AbisoIP</v>
-      </c>
-      <c r="E7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E7" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Traffic Check for Traffic shiftng</v>
-      </c>
-      <c r="F7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>HGNBG28,HGNBG08</v>
-      </c>
-      <c r="G7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G7" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H7" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
-      </c>
-      <c r="J7" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J7" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
+        <v>0</v>
       </c>
       <c r="K7" s="31"/>
-      <c r="L7" s="31" t="str">
+      <c r="L7" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B8" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44076</v>
-      </c>
-      <c r="C8" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C8" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D8" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>DHAKA_MODERNIZATION</v>
-      </c>
-      <c r="E8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E8" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>HW upgradation</v>
-      </c>
-      <c r="F8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F8" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>GPSDR86,GPSDR42</v>
-      </c>
-      <c r="G8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G8" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H8" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I8" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J8" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J8" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka North</v>
+        <v>0</v>
       </c>
       <c r="K8" s="31"/>
-      <c r="L8" s="31" t="str">
+      <c r="L8" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B9" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44076</v>
-      </c>
-      <c r="C9" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C9" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
-      </c>
-      <c r="D9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D9" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
-      </c>
-      <c r="E9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E9" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Configuration</v>
-      </c>
-      <c r="F9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F9" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHDHN45,DHKHL47,DHKHLA0,DHPTN29,DHRMN04,DHRMN16,DHRMN26,DHBDD78,DHGULF5,DHMDP01</v>
-      </c>
-      <c r="G9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G9" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H9" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I9" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J9" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J9" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>0</v>
       </c>
       <c r="K9" s="31"/>
-      <c r="L9" s="31" t="str">
+      <c r="L9" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B10" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44076</v>
-      </c>
-      <c r="C10" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="C10" s="29">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
-      </c>
-      <c r="D10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="D10" s="30">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
-      </c>
-      <c r="E10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="E10" s="30">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Configuration</v>
-      </c>
-      <c r="F10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="F10" s="30">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>MGGHR11,MGSBL11,MGSTR01,MNLHG02,MNLHG17,GPSDRS5,MNSDR46,DHSVRG5</v>
-      </c>
-      <c r="G10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="G10" s="30">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="H10" s="30">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="I10" s="30">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J10" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="J10" s="30">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka North</v>
+        <v>0</v>
       </c>
       <c r="K10" s="31"/>
-      <c r="L10" s="31" t="str">
+      <c r="L10" s="31">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Locators has been fully transfered
</commit_message>
<xml_diff>
--- a/data_driver/Change_Requirement.xlsx
+++ b/data_driver/Change_Requirement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\AutoBotBMCRemedy\data_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3847D56E-C634-4F14-9315-C98737E82744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97BCA1-3FDC-4B9C-9115-1D27FF21FF53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1493,7 +1493,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,44 +1557,44 @@
       </c>
       <c r="B2" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
+        <v>44095</v>
       </c>
       <c r="C2" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Shahadat Hossain</v>
+        <v>Md. Rashekul Islam Raju</v>
       </c>
       <c r="D2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>CC 4G Colocation Project</v>
+        <v>MW antenna optimization</v>
       </c>
       <c r="E2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>GSM Antenna &amp; RRU Swap</v>
+        <v>MW antenna optimization</v>
       </c>
       <c r="F2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>LXRGN14,LXRGN11,LXRGN33,LXRPR19</v>
+        <v>DHGUL11, DHGUL26, DHGUL74</v>
       </c>
       <c r="G2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
+        <v>Non-Service Effective</v>
       </c>
       <c r="H2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>04:00 Hour</v>
+        <v>00:45 Minute</v>
       </c>
       <c r="I2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Noakhali</v>
+        <v>Dhaka</v>
       </c>
       <c r="J2" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Noakhali</v>
+        <v>e.co_Dhaka Metro</v>
       </c>
       <c r="K2" s="31"/>
       <c r="L2" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Faisal Mahmud Fuad</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1604,23 +1604,23 @@
       </c>
       <c r="B3" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
+        <v>44095</v>
       </c>
       <c r="C3" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Shahadat Hossain</v>
+        <v>Prodip Biswas</v>
       </c>
       <c r="D3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>CC 4G Colocation Project</v>
+        <v>L18CellAdd, Y2020</v>
       </c>
       <c r="E3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>GSM Antenna &amp; RRU Swap</v>
+        <v>GSM &amp; RRU Swap</v>
       </c>
       <c r="F3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>BMAKH14,BMNBG17,BMNBG19,BMNBG23</v>
+        <v>   MBKLR26, SYBLG20</v>
       </c>
       <c r="G3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
@@ -1628,20 +1628,20 @@
       </c>
       <c r="H3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>04:00 Hour</v>
+        <v>00:30 Minute</v>
       </c>
       <c r="I3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Comilla</v>
+        <v>Sylhet</v>
       </c>
       <c r="J3" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Comilla</v>
+        <v>e.co_Sylhet</v>
       </c>
       <c r="K3" s="31"/>
       <c r="L3" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Faisal Mahmud Fuad</v>
+        <v>Sumon Kumar Biswas</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1651,39 +1651,39 @@
       </c>
       <c r="B4" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
+        <v>44095</v>
       </c>
       <c r="C4" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Rashekul Islam Raju</v>
+        <v>Md. Masudur Rahman</v>
       </c>
       <c r="D4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>MW antenna optimization</v>
+        <v>NCCD AbisoIP</v>
       </c>
       <c r="E4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>MW antenna optimization</v>
+        <v>Rectification</v>
       </c>
       <c r="F4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHKTL29, DHKTL62, DHPTN08, DHKHL74</v>
+        <v>SYZKG15,SYZKG01</v>
       </c>
       <c r="G4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
+        <v>Service Effective</v>
       </c>
       <c r="H4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:45 Minute</v>
+        <v>00:30 Minute</v>
       </c>
       <c r="I4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
+        <v>Sylhet</v>
       </c>
       <c r="J4" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>e.co_Sylhet</v>
       </c>
       <c r="K4" s="31"/>
       <c r="L4" s="31" t="str">
@@ -1698,44 +1698,44 @@
       </c>
       <c r="B5" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
+        <v>44095</v>
       </c>
       <c r="C5" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Prodip Biswas</v>
+        <v>Md. Masudur Rahman</v>
       </c>
       <c r="D5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>L18CellAdd, Y2020</v>
+        <v>DHAKA_MODERNIZATION</v>
       </c>
       <c r="E5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>GSM &amp; RRU Swap</v>
+        <v>DCN Configure</v>
       </c>
       <c r="F5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>   SYBNC02,MBKLR26</v>
+        <v>NGARH26,NGARH09,NGSNG11,NGSNG20</v>
       </c>
       <c r="G5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
+        <v>Non-Service Effective</v>
       </c>
       <c r="H5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
+        <v>00:00 Minute</v>
       </c>
       <c r="I5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
+        <v>Dhaka</v>
       </c>
       <c r="J5" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
+        <v>e.co_Dhaka South</v>
       </c>
       <c r="K5" s="31"/>
       <c r="L5" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Sumon Kumar Biswas</v>
+        <v>Muhammad Shahed</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1745,39 +1745,39 @@
       </c>
       <c r="B6" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
+        <v>44095</v>
       </c>
       <c r="C6" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
+        <v>Md. Masudur Rahman</v>
       </c>
       <c r="D6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
+        <v>DHAKA_MODERNIZATION</v>
       </c>
       <c r="E6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Ping Test</v>
+        <v>Rectification for XPIC allignment</v>
       </c>
       <c r="F6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>GPSDR76,GPSDRN0,MGSDR31,MNLHG11,MNSDR19,MNSDR28,MNSRN16,MNSRN17,GPKLK27,GPSDR61</v>
+        <v>TNGPL01,TNGTL27</v>
       </c>
       <c r="G6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
+        <v>Service Effective</v>
       </c>
       <c r="H6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
+        <v>00:30 Minute</v>
       </c>
       <c r="I6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
+        <v>Mymensingh</v>
       </c>
       <c r="J6" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka North</v>
+        <v>e.co_Mymensingh</v>
       </c>
       <c r="K6" s="31"/>
       <c r="L6" s="31" t="str">
@@ -1792,23 +1792,23 @@
       </c>
       <c r="B7" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
+        <v>44095</v>
       </c>
       <c r="C7" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
+        <v>Md. Masudur Rahman</v>
       </c>
       <c r="D7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
+        <v>DHAKA_MODERNIZATION</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Ping Test</v>
+        <v>Ne link installation</v>
       </c>
       <c r="F7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>DHBDD05,DHDHN45,DHMJH47,DHPTN16,DHRMN36,DHBDD78,DHGULF5,DHMDP01,DHMDP05</v>
+        <v>GPKLG05,GPSDR06,DHKHGT1,MGSNG08</v>
       </c>
       <c r="G7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="J7" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka Metro</v>
+        <v>e.co_Dhaka North</v>
       </c>
       <c r="K7" s="31"/>
       <c r="L7" s="31" t="str">
@@ -1839,23 +1839,28 @@
       </c>
       <c r="B8" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
+        <v>44095</v>
       </c>
       <c r="C8" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>KM Jiaul Islam Jibon</v>
+        <v>Md. Masudur Rahman</v>
       </c>
       <c r="D8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Dhaka-Modernization</v>
+        <v>Padma_Colo</v>
       </c>
       <c r="E8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>FE Ping Test</v>
+        <v>MW Dismantle activity
+Link ID:SY13H31786
+Link Name:SYBNB22-SYBNB26
+DCN Impact:SYBNB26-EMTN-01,SYBNB22-EMTN-01,SYBNB22-EMTN-01,SYBNB29-EMTN-01
+DCN Path:SYBNB26-SYBNB22-SYBNB05-SYBNB29
+Impact list:SYBNB22,SYBNB26</v>
       </c>
       <c r="F8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>TNGPL06</v>
+        <v>SYBNB22,SYBNB26</v>
       </c>
       <c r="G8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
@@ -1867,11 +1872,11 @@
       </c>
       <c r="I8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Mymensingh</v>
+        <v>Sylhet</v>
       </c>
       <c r="J8" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Mymensingh</v>
+        <v>e.co_Sylhet</v>
       </c>
       <c r="K8" s="31"/>
       <c r="L8" s="31" t="str">
@@ -1886,7 +1891,7 @@
       </c>
       <c r="B9" s="28">
         <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
+        <v>44095</v>
       </c>
       <c r="C9" s="29" t="str">
         <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
@@ -1894,253 +1899,9 @@
       </c>
       <c r="D9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>NCCD AbisoIP</v>
+        <v>Padma_Colo</v>
       </c>
       <c r="E9" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Rectification</v>
-      </c>
-      <c r="F9" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>SYZKG15,SYZKG01</v>
-      </c>
-      <c r="G9" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H9" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I9" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
-      </c>
-      <c r="J9" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
-      </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31" t="str">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
-        <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>9</v>
-      </c>
-      <c r="B10" s="28">
-        <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
-      </c>
-      <c r="C10" s="29" t="str">
-        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D10" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>DHAKA_MODERNIZATION</v>
-      </c>
-      <c r="E10" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>DCN Configure</v>
-      </c>
-      <c r="F10" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>NGARH26,NGARH09</v>
-      </c>
-      <c r="G10" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Non-Service Effective</v>
-      </c>
-      <c r="H10" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:00 Minute</v>
-      </c>
-      <c r="I10" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J10" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka South</v>
-      </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31" t="str">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
-        <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>10</v>
-      </c>
-      <c r="B11" s="28">
-        <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
-      </c>
-      <c r="C11" s="29" t="str">
-        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D11" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>DHAKA_MODERNIZATION</v>
-      </c>
-      <c r="E11" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>Link ID:DH07E18275
-Link Name:MNLHG18-MNSRN18
-DCN Impact:MNLHG18-EMTN-02,MNLHG18-EMTN-01,MNLHG02-EMTN-01,MNLHG08-EMTN-01,MNLHG18-EMTN-03,MNSRN18-EMTN-02
-DCN Path:MNSRN18-MNLHG18-MNLHG02,MNLHG08
-Impact List:MNLHG18,MNSRN18</v>
-      </c>
-      <c r="F11" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>MNLHG18,MNSRN18</v>
-      </c>
-      <c r="G11" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H11" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I11" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J11" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka South</v>
-      </c>
-      <c r="K11" s="32"/>
-      <c r="L11" s="31" t="str">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
-        <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>11</v>
-      </c>
-      <c r="B12" s="28">
-        <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
-      </c>
-      <c r="C12" s="29" t="str">
-        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D12" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>DHAKA_MODERNIZATION</v>
-      </c>
-      <c r="E12" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>New link installation</v>
-      </c>
-      <c r="F12" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>GPKLG05,GPSDR06,DHKHGT1,MGSNG08</v>
-      </c>
-      <c r="G12" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H12" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I12" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Dhaka</v>
-      </c>
-      <c r="J12" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Dhaka North</v>
-      </c>
-      <c r="K12" s="32"/>
-      <c r="L12" s="31" t="str">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
-        <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>12</v>
-      </c>
-      <c r="B13" s="28">
-        <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
-      </c>
-      <c r="C13" s="29" t="str">
-        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D13" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Padma_Colo</v>
-      </c>
-      <c r="E13" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
-        <v>MW Dismantle activity
-Link ID:SY07H30744
-Link Name:SNDKS01-SNDRI01
-DCN Impact:SNDKS01-HRTN-01,SNDKS01-HRTN-02,SNDKS01-HRTN-03,SNDRI01-HRTN01
-DCN Path:SNJML02-SNDKS01-SNDRI05
-Impact list:SNDKS01,SNDRI01,SNDRI10</v>
-      </c>
-      <c r="F13" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
-        <v>SNDKS01,SNDRI01</v>
-      </c>
-      <c r="G13" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Service Type]]</f>
-        <v>Service Effective</v>
-      </c>
-      <c r="H13" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Down Time]]</f>
-        <v>00:30 Minute</v>
-      </c>
-      <c r="I13" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
-      </c>
-      <c r="J13" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
-      </c>
-      <c r="K13" s="32"/>
-      <c r="L13" s="31" t="str">
-        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
-        <v>Muhammad Shahed</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
-        <f>[1]!Table1[[#This Row],[No]]</f>
-        <v>13</v>
-      </c>
-      <c r="B14" s="28">
-        <f>[1]!Table1[[#This Row],[Date]]</f>
-        <v>44093</v>
-      </c>
-      <c r="C14" s="29" t="str">
-        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
-        <v>Md. Masudur Rahman</v>
-      </c>
-      <c r="D14" s="30" t="str">
-        <f>[1]!Table1[[#This Row],[Project Name]]</f>
-        <v>Padma_Colo</v>
-      </c>
-      <c r="E14" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Change Activity]]</f>
         <v>MW Dismantle activity
 Link ID:SY07H30739
@@ -2148,30 +1909,265 @@
 DCN Impact: SNDRI01-HRTN01,SNDRI01-HRTN02
 DCN Path:SNDRI01-SNDRI10</v>
       </c>
-      <c r="F14" s="30" t="str">
+      <c r="F9" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
         <v>SNDRI01,SNDRI10</v>
       </c>
-      <c r="G14" s="30" t="str">
+      <c r="G9" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Service Type]]</f>
+        <v>Non-Service Effective</v>
+      </c>
+      <c r="H9" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Down Time]]</f>
+        <v>00:00 Minute</v>
+      </c>
+      <c r="I9" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Site Group]]</f>
+        <v>Sylhet</v>
+      </c>
+      <c r="J9" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
+        <v>e.co_Sylhet</v>
+      </c>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31" t="str">
+        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
+        <v>Muhammad Shahed</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
+        <f>[1]!Table1[[#This Row],[No]]</f>
+        <v>9</v>
+      </c>
+      <c r="B10" s="28">
+        <f>[1]!Table1[[#This Row],[Date]]</f>
+        <v>44095</v>
+      </c>
+      <c r="C10" s="29" t="str">
+        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
+        <v>KM Jiaul Islam Jibon</v>
+      </c>
+      <c r="D10" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Project Name]]</f>
+        <v>Dhaka-Modernization</v>
+      </c>
+      <c r="E10" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
+        <v>FE Configuration</v>
+      </c>
+      <c r="F10" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
+        <v>MGDLP08</v>
+      </c>
+      <c r="G10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Service Type]]</f>
         <v>Service Effective</v>
       </c>
-      <c r="H14" s="30" t="str">
+      <c r="H10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Down Time]]</f>
         <v>00:30 Minute</v>
       </c>
-      <c r="I14" s="30" t="str">
+      <c r="I10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Site Group]]</f>
-        <v>Sylhet</v>
-      </c>
-      <c r="J14" s="30" t="str">
+        <v>Dhaka</v>
+      </c>
+      <c r="J10" s="30" t="str">
         <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
-        <v>e.co_Sylhet</v>
-      </c>
-      <c r="K14" s="32"/>
-      <c r="L14" s="31" t="str">
+        <v>e.co_Dhaka North</v>
+      </c>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31" t="str">
         <f>[1]!Table1[[#This Row],[Change Manager]]</f>
         <v>Muhammad Shahed</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27">
+        <f>[1]!Table1[[#This Row],[No]]</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="28">
+        <f>[1]!Table1[[#This Row],[Date]]</f>
+        <v>44095</v>
+      </c>
+      <c r="C11" s="29" t="str">
+        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
+        <v>Md. Shahadat Hossain</v>
+      </c>
+      <c r="D11" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Project Name]]</f>
+        <v>CC 4G Colocation Project</v>
+      </c>
+      <c r="E11" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
+        <v>GSM Antenna &amp; RRU Swap</v>
+      </c>
+      <c r="F11" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
+        <v>LXRGN14,LXRGN11,LXRPR19</v>
+      </c>
+      <c r="G11" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Service Type]]</f>
+        <v>Service Effective</v>
+      </c>
+      <c r="H11" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Down Time]]</f>
+        <v>04:00 Hour</v>
+      </c>
+      <c r="I11" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Site Group]]</f>
+        <v>Noakhali</v>
+      </c>
+      <c r="J11" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
+        <v>e.co_Noakhali</v>
+      </c>
+      <c r="K11" s="32"/>
+      <c r="L11" s="31" t="str">
+        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
+        <v>Faisal Mahmud Fuad</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <f>[1]!Table1[[#This Row],[No]]</f>
+        <v>11</v>
+      </c>
+      <c r="B12" s="28">
+        <f>[1]!Table1[[#This Row],[Date]]</f>
+        <v>44095</v>
+      </c>
+      <c r="C12" s="29" t="str">
+        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
+        <v>Md. Shahadat Hossain</v>
+      </c>
+      <c r="D12" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Project Name]]</f>
+        <v>CC 4G Colocation Project</v>
+      </c>
+      <c r="E12" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
+        <v>GSM Antenna &amp; RRU Swap</v>
+      </c>
+      <c r="F12" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
+        <v>BMNBG17,BMNBG19</v>
+      </c>
+      <c r="G12" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Service Type]]</f>
+        <v>Service Effective</v>
+      </c>
+      <c r="H12" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Down Time]]</f>
+        <v>04:00 Hour</v>
+      </c>
+      <c r="I12" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Site Group]]</f>
+        <v>Comilla</v>
+      </c>
+      <c r="J12" s="30" t="str">
+        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
+        <v>e.co_Comilla</v>
+      </c>
+      <c r="K12" s="32"/>
+      <c r="L12" s="31" t="str">
+        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
+        <v>Faisal Mahmud Fuad</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <f>[1]!Table1[[#This Row],[No]]</f>
+        <v>0</v>
+      </c>
+      <c r="B13" s="28">
+        <f>[1]!Table1[[#This Row],[Date]]</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="29">
+        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="30">
+        <f>[1]!Table1[[#This Row],[Project Name]]</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="30">
+        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="30">
+        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="30">
+        <f>[1]!Table1[[#This Row],[Service Type]]</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="30">
+        <f>[1]!Table1[[#This Row],[Down Time]]</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="30">
+        <f>[1]!Table1[[#This Row],[Site Group]]</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="30">
+        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="32"/>
+      <c r="L13" s="31">
+        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
+        <f>[1]!Table1[[#This Row],[No]]</f>
+        <v>0</v>
+      </c>
+      <c r="B14" s="28">
+        <f>[1]!Table1[[#This Row],[Date]]</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="29">
+        <f>[1]!Table1[[#This Row],[Project Coordinator]]</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="30">
+        <f>[1]!Table1[[#This Row],[Project Name]]</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="30">
+        <f>[1]!Table1[[#This Row],[Change Activity]]</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="30">
+        <f>[1]!Table1[[#This Row],[Impact Site List]]</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="30">
+        <f>[1]!Table1[[#This Row],[Service Type]]</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="30">
+        <f>[1]!Table1[[#This Row],[Down Time]]</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="30">
+        <f>[1]!Table1[[#This Row],[Site Group]]</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="30">
+        <f>[1]!Table1[[#This Row],[Commercial Zone]]</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="32"/>
+      <c r="L14" s="31">
+        <f>[1]!Table1[[#This Row],[Change Manager]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>